<commit_message>
momentary mass at start of motions
</commit_message>
<xml_diff>
--- a/Post_Flight_Datasheet_03_05_V4 (1).xlsx
+++ b/Post_Flight_Datasheet_03_05_V4 (1).xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stein\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F47B0D4-AF8B-4A1B-A6C3-E69A6158F299}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="79">
   <si>
     <t>Post-Flight Data Sheet AE3202</t>
   </si>
@@ -223,9 +223,6 @@
     <t>zesenveertig50</t>
   </si>
   <si>
-    <t>vierenvijftig30</t>
-  </si>
-  <si>
     <t>Daan</t>
   </si>
   <si>
@@ -239,12 +236,33 @@
   </si>
   <si>
     <t>Nick</t>
+  </si>
+  <si>
+    <t>vierenvijftig40</t>
+  </si>
+  <si>
+    <t>vijfenveertig47</t>
+  </si>
+  <si>
+    <t>time elapsed</t>
+  </si>
+  <si>
+    <t>momentary mass</t>
+  </si>
+  <si>
+    <t>[kg]</t>
+  </si>
+  <si>
+    <t>mass flow</t>
+  </si>
+  <si>
+    <t>[lbs/sec]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -265,12 +283,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -306,9 +330,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,8 +450,58 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5228640" y="987480"/>
-          <a:ext cx="2424240" cy="3332520"/>
+          <a:off x="4501785" y="987780"/>
+          <a:ext cx="1830315" cy="3332460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>491760</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>426600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>129240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5511435" y="987780"/>
+          <a:ext cx="2373240" cy="3332460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -703,29 +778,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M84" sqref="A1:M84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7"/>
-    <col min="14" max="1025" width="8.5546875"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -737,7 +809,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -749,13 +821,13 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -763,7 +835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -772,7 +844,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -781,7 +853,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -790,62 +862,62 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H12" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H13" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H14" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -856,20 +928,20 @@
         <v>94.5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -877,7 +949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -909,7 +981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
@@ -938,7 +1010,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -970,7 +1042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1002,7 +1074,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1034,7 +1106,7 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1066,7 +1138,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1098,7 +1170,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1130,7 +1202,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1144,23 +1216,23 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1192,7 +1264,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>42</v>
       </c>
@@ -1221,7 +1293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1235,7 +1307,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1249,7 +1321,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1263,7 +1335,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1277,7 +1349,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1291,7 +1363,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6</v>
       </c>
@@ -1305,7 +1377,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -1319,17 +1391,17 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1337,7 +1409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -1378,7 +1450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>42</v>
       </c>
@@ -1416,7 +1488,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1457,7 +1529,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1496,7 +1568,7 @@
         <v>-4.9000000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -1535,7 +1607,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -1574,7 +1646,7 @@
         <v>-6.5</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5</v>
       </c>
@@ -1613,7 +1685,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>6</v>
       </c>
@@ -1652,7 +1724,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7</v>
       </c>
@@ -1691,17 +1763,17 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -1709,7 +1781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>50</v>
       </c>
@@ -1723,7 +1795,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>21</v>
       </c>
@@ -1764,7 +1836,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>42</v>
       </c>
@@ -1802,7 +1874,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1841,7 +1913,7 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -1880,17 +1952,17 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
         <v>53</v>
       </c>
@@ -1901,7 +1973,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
         <v>42</v>
       </c>
@@ -1912,7 +1984,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>54</v>
       </c>
@@ -1929,10 +2001,10 @@
         <v>56</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>57</v>
       </c>
@@ -1948,87 +2020,89 @@
       <c r="H84" t="s">
         <v>59</v>
       </c>
-      <c r="J84" s="5"/>
+      <c r="J84" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <conditionalFormatting sqref="B34:J34 D28:J31 B28:B31">
-    <cfRule type="expression" priority="3">
+    <cfRule type="expression" priority="1">
       <formula>LEN(TRIM(B28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" priority="4">
+    <cfRule type="expression" priority="2">
       <formula>LEN(TRIM(D18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:J33">
-    <cfRule type="expression" priority="5">
+    <cfRule type="expression" priority="3">
       <formula>LEN(TRIM(B32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:M65">
-    <cfRule type="expression" priority="6">
+    <cfRule type="expression" priority="4">
       <formula>LEN(TRIM(C59))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:J50">
-    <cfRule type="expression" priority="7">
+    <cfRule type="expression" priority="5">
       <formula>LEN(TRIM(C44))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" priority="8">
+    <cfRule type="expression" priority="6">
       <formula>LEN(TRIM(C70))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="expression" priority="9">
+    <cfRule type="expression" priority="7">
       <formula>LEN(TRIM(C71))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="expression" priority="10">
+    <cfRule type="expression" priority="8">
       <formula>LEN(TRIM(H71))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:M76">
-    <cfRule type="expression" priority="11">
+    <cfRule type="expression" priority="9">
       <formula>LEN(TRIM(B75))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D4">
-    <cfRule type="expression" priority="12">
+    <cfRule type="expression" priority="10">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" priority="13">
+    <cfRule type="expression" priority="11">
       <formula>LEN(TRIM(E39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:D84">
-    <cfRule type="expression" priority="14">
+    <cfRule type="expression" priority="12">
       <formula>LEN(TRIM(D83))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83:G84">
-    <cfRule type="expression" priority="15">
+    <cfRule type="expression" priority="13">
       <formula>LEN(TRIM(G83))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83:J84">
-    <cfRule type="expression" priority="16">
+    <cfRule type="expression" priority="14">
       <formula>LEN(TRIM(J83))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59:B65">
-    <cfRule type="expression" priority="17">
+    <cfRule type="expression" priority="15">
       <formula>LEN(TRIM(B59))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:B50">
-    <cfRule type="expression" priority="18">
+    <cfRule type="expression" priority="16">
       <formula>LEN(TRIM(B44))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2036,4 +2110,1401 @@
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>43529</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="H8" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="H9" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="H10" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="2">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1120</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E28" s="2">
+        <v>250</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="G28" s="2">
+        <v>732</v>
+      </c>
+      <c r="H28" s="2">
+        <v>777</v>
+      </c>
+      <c r="I28" s="2">
+        <v>405</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.84305555555555556</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1214</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E29" s="2">
+        <v>219</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>605</v>
+      </c>
+      <c r="H29" s="2">
+        <v>650</v>
+      </c>
+      <c r="I29" s="2">
+        <v>440</v>
+      </c>
+      <c r="J29" s="2">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.91041666666666676</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1311</v>
+      </c>
+      <c r="D30" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E30" s="2">
+        <v>190</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="G30" s="2">
+        <v>506</v>
+      </c>
+      <c r="H30" s="2">
+        <v>546</v>
+      </c>
+      <c r="I30" s="2">
+        <v>469</v>
+      </c>
+      <c r="J30" s="2">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1.0194444444444444</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1468</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E31" s="2">
+        <v>160</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>421</v>
+      </c>
+      <c r="H31" s="2">
+        <v>473</v>
+      </c>
+      <c r="I31" s="2">
+        <v>500</v>
+      </c>
+      <c r="J31" s="2">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1.1104166666666666</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1599</v>
+      </c>
+      <c r="D32" s="2">
+        <v>8010</v>
+      </c>
+      <c r="E32" s="2">
+        <v>132</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="G32" s="2">
+        <v>410</v>
+      </c>
+      <c r="H32" s="2">
+        <v>444</v>
+      </c>
+      <c r="I32" s="2">
+        <v>530</v>
+      </c>
+      <c r="J32" s="2">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1.2013888888888888</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1730</v>
+      </c>
+      <c r="D33" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E33" s="2">
+        <v>114</v>
+      </c>
+      <c r="F33" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>397</v>
+      </c>
+      <c r="H33" s="2">
+        <v>430</v>
+      </c>
+      <c r="I33" s="2">
+        <v>555</v>
+      </c>
+      <c r="J33" s="2">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56" t="s">
+        <v>44</v>
+      </c>
+      <c r="H56" t="s">
+        <v>45</v>
+      </c>
+      <c r="I56" t="s">
+        <v>46</v>
+      </c>
+      <c r="J56" t="s">
+        <v>27</v>
+      </c>
+      <c r="K56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" t="s">
+        <v>29</v>
+      </c>
+      <c r="M56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" s="5">
+        <v>33.159999999999997</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1996</v>
+      </c>
+      <c r="D59" s="2">
+        <v>7970</v>
+      </c>
+      <c r="E59" s="2">
+        <v>161</v>
+      </c>
+      <c r="F59" s="2">
+        <v>5</v>
+      </c>
+      <c r="G59" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="H59" s="2">
+        <v>2</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2">
+        <v>412</v>
+      </c>
+      <c r="K59" s="2">
+        <v>446</v>
+      </c>
+      <c r="L59" s="2">
+        <v>620</v>
+      </c>
+      <c r="M59" s="2">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="2">
+        <v>2072</v>
+      </c>
+      <c r="D60" s="2">
+        <v>8120</v>
+      </c>
+      <c r="E60" s="2">
+        <v>150</v>
+      </c>
+      <c r="F60" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="G60" s="2">
+        <v>-0.9</v>
+      </c>
+      <c r="H60" s="2">
+        <v>2</v>
+      </c>
+      <c r="I60" s="2">
+        <v>-16</v>
+      </c>
+      <c r="J60" s="2">
+        <v>409</v>
+      </c>
+      <c r="K60" s="2">
+        <v>443</v>
+      </c>
+      <c r="L60" s="2">
+        <v>642</v>
+      </c>
+      <c r="M60" s="2">
+        <v>-4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="2">
+        <v>2150</v>
+      </c>
+      <c r="D61" s="2">
+        <v>8350</v>
+      </c>
+      <c r="E61" s="2">
+        <v>140</v>
+      </c>
+      <c r="F61" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="G61" s="2">
+        <v>-1.4</v>
+      </c>
+      <c r="H61" s="2">
+        <v>2</v>
+      </c>
+      <c r="I61" s="2">
+        <v>-29</v>
+      </c>
+      <c r="J61" s="2">
+        <v>406</v>
+      </c>
+      <c r="K61" s="2">
+        <v>440</v>
+      </c>
+      <c r="L61" s="2">
+        <v>658</v>
+      </c>
+      <c r="M61" s="2">
+        <v>-5.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="2">
+        <v>2222</v>
+      </c>
+      <c r="D62" s="2">
+        <v>8550</v>
+      </c>
+      <c r="E62" s="2">
+        <v>131</v>
+      </c>
+      <c r="F62" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="G62" s="2">
+        <v>-2</v>
+      </c>
+      <c r="H62" s="2">
+        <v>2</v>
+      </c>
+      <c r="I62" s="2">
+        <v>-41</v>
+      </c>
+      <c r="J62" s="2">
+        <v>402</v>
+      </c>
+      <c r="K62" s="2">
+        <v>433</v>
+      </c>
+      <c r="L62" s="2">
+        <v>675</v>
+      </c>
+      <c r="M62" s="2">
+        <v>-6.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="2">
+        <v>2358</v>
+      </c>
+      <c r="D63" s="2">
+        <v>7800</v>
+      </c>
+      <c r="E63" s="2">
+        <v>170</v>
+      </c>
+      <c r="F63" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="G63" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="H63" s="2">
+        <v>2</v>
+      </c>
+      <c r="I63" s="2">
+        <v>-19</v>
+      </c>
+      <c r="J63" s="2">
+        <v>416</v>
+      </c>
+      <c r="K63" s="2">
+        <v>452</v>
+      </c>
+      <c r="L63" s="2">
+        <v>708</v>
+      </c>
+      <c r="M63" s="2">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>6</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="2">
+        <v>2430</v>
+      </c>
+      <c r="D64" s="2">
+        <v>7320</v>
+      </c>
+      <c r="E64" s="2">
+        <v>181</v>
+      </c>
+      <c r="F64" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H64" s="2">
+        <v>2</v>
+      </c>
+      <c r="I64" s="2">
+        <v>40</v>
+      </c>
+      <c r="J64" s="2">
+        <v>424</v>
+      </c>
+      <c r="K64" s="2">
+        <v>460</v>
+      </c>
+      <c r="L64" s="2">
+        <v>726</v>
+      </c>
+      <c r="M64" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>7</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="2">
+        <v>2516</v>
+      </c>
+      <c r="D65" s="2">
+        <v>6850</v>
+      </c>
+      <c r="E65" s="2">
+        <v>188</v>
+      </c>
+      <c r="F65" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2</v>
+      </c>
+      <c r="I65" s="2">
+        <v>51</v>
+      </c>
+      <c r="J65" s="2">
+        <v>433</v>
+      </c>
+      <c r="K65" s="2">
+        <v>468</v>
+      </c>
+      <c r="L65" s="2">
+        <v>740</v>
+      </c>
+      <c r="M65" s="2">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E71" t="s">
+        <v>51</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" t="s">
+        <v>44</v>
+      </c>
+      <c r="H73" t="s">
+        <v>45</v>
+      </c>
+      <c r="I73" t="s">
+        <v>46</v>
+      </c>
+      <c r="J73" t="s">
+        <v>27</v>
+      </c>
+      <c r="K73" t="s">
+        <v>28</v>
+      </c>
+      <c r="L73" t="s">
+        <v>29</v>
+      </c>
+      <c r="M73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M74" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="2">
+        <v>2595</v>
+      </c>
+      <c r="D75" s="2">
+        <v>7100</v>
+      </c>
+      <c r="E75" s="2">
+        <v>158</v>
+      </c>
+      <c r="F75" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G75" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="H75" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="I75" s="2">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2">
+        <v>422</v>
+      </c>
+      <c r="K75" s="2">
+        <v>458</v>
+      </c>
+      <c r="L75" s="2">
+        <v>767</v>
+      </c>
+      <c r="M75" s="2">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="2">
+        <v>2680</v>
+      </c>
+      <c r="D76" s="2">
+        <v>7090</v>
+      </c>
+      <c r="E76" s="2">
+        <v>159</v>
+      </c>
+      <c r="F76" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G76" s="2">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H76" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="I76" s="2">
+        <v>-25</v>
+      </c>
+      <c r="J76" s="2">
+        <v>422</v>
+      </c>
+      <c r="K76" s="2">
+        <v>458</v>
+      </c>
+      <c r="L76" s="2">
+        <v>788</v>
+      </c>
+      <c r="M76" s="2">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" t="s">
+        <v>53</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G81" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" t="s">
+        <v>42</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83">
+        <f>45*60+47</f>
+        <v>2747</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="8">
+        <f>($D$18-$L$76-$G$83*(C83-$C$76)+11053.1)*0.453592</f>
+        <v>5896.0839415641021</v>
+      </c>
+      <c r="G83">
+        <f>(L76-I28)/(C76-C28)</f>
+        <v>0.2455128205128205</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84">
+        <f>46*60+50</f>
+        <v>2810</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E84" s="8">
+        <f t="shared" ref="E84:E88" si="0">($D$18-$L$76-$G$83*(C84-$C$76)+11053.1)*0.453592</f>
+        <v>5889.0680945333334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C85">
+        <f>47*60+40</f>
+        <v>2860</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="8">
+        <f t="shared" si="0"/>
+        <v>5883.4999619692317</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86">
+        <f>51*60+3</f>
+        <v>3063</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" s="8">
+        <f t="shared" si="0"/>
+        <v>5860.8933437589749</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>58</v>
+      </c>
+      <c r="C87">
+        <f>52*60+3</f>
+        <v>3123</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E87" s="8">
+        <f t="shared" si="0"/>
+        <v>5854.2115846820516</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>59</v>
+      </c>
+      <c r="C88">
+        <f>54*60+40</f>
+        <v>3280</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E88" s="8">
+        <f t="shared" si="0"/>
+        <v>5836.7276484307686</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A83:D88">
+    <sortCondition ref="C83:C88"/>
+  </sortState>
+  <conditionalFormatting sqref="B34:J34 D28:J31 B28:B31">
+    <cfRule type="expression" priority="1">
+      <formula>LEN(TRIM(B28))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="expression" priority="2">
+      <formula>LEN(TRIM(D18))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:J33">
+    <cfRule type="expression" priority="3">
+      <formula>LEN(TRIM(B32))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:M65">
+    <cfRule type="expression" priority="4">
+      <formula>LEN(TRIM(C59))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:J50">
+    <cfRule type="expression" priority="5">
+      <formula>LEN(TRIM(C44))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70">
+    <cfRule type="expression" priority="6">
+      <formula>LEN(TRIM(C70))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71">
+    <cfRule type="expression" priority="7">
+      <formula>LEN(TRIM(C71))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71">
+    <cfRule type="expression" priority="8">
+      <formula>LEN(TRIM(H71))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75:M76">
+    <cfRule type="expression" priority="9">
+      <formula>LEN(TRIM(B75))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="expression" priority="10">
+      <formula>LEN(TRIM(D3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" priority="11">
+      <formula>LEN(TRIM(E39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D83:D84">
+    <cfRule type="expression" priority="12">
+      <formula>LEN(TRIM(D83))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D85:D86">
+    <cfRule type="expression" priority="13">
+      <formula>LEN(TRIM(D85))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D88">
+    <cfRule type="expression" priority="14">
+      <formula>LEN(TRIM(D87))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59:B65">
+    <cfRule type="expression" priority="15">
+      <formula>LEN(TRIM(B59))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44:B50">
+    <cfRule type="expression" priority="16">
+      <formula>LEN(TRIM(B44))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>